<commit_message>
Added 2 new versions. Improved recognition with noise. Increase start silence threshold. Added 2 new voice commands!
</commit_message>
<xml_diff>
--- a/Audio Dataset Stats.xlsx
+++ b/Audio Dataset Stats.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cipri\Desktop\voice recognition\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\_Middlesex University\Third Year\PDE3400 Design Engineering Major Project\Development\voice recognition\long_commands_cnn\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7E974B5-FE48-4AE1-A4B6-5D467FC49EAC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2725D6CA-92C5-4A58-BA87-41BF5B57A599}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="77040" windowHeight="21840" xr2:uid="{F11276A6-3647-4A1C-99D0-FA80B05CBAB3}"/>
+    <workbookView xWindow="27345" yWindow="165" windowWidth="34590" windowHeight="19395" xr2:uid="{F11276A6-3647-4A1C-99D0-FA80B05CBAB3}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,14 +35,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="37">
   <si>
     <t>Total Samples:</t>
   </si>
   <si>
-    <t>15 000</t>
-  </si>
-  <si>
     <t>Samples per class:</t>
   </si>
   <si>
@@ -52,9 +49,6 @@
     <t>Total audio time:</t>
   </si>
   <si>
-    <t>5h 33m 9s</t>
-  </si>
-  <si>
     <t>AUDIO TIME PER CLASS</t>
   </si>
   <si>
@@ -134,6 +128,24 @@
   </si>
   <si>
     <t>IN SECONDS:</t>
+  </si>
+  <si>
+    <t>6h 30m 34s</t>
+  </si>
+  <si>
+    <t>AIR QUALITY</t>
+  </si>
+  <si>
+    <t>25m 17s</t>
+  </si>
+  <si>
+    <t>32m 8s</t>
+  </si>
+  <si>
+    <t>17 500</t>
+  </si>
+  <si>
+    <t>ATMOSPHERE</t>
   </si>
 </sst>
 </file>
@@ -226,8 +238,8 @@
           <c:layoutTarget val="inner"/>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.28315281056654273"/>
-          <c:y val="5.6846460083772178E-2"/>
+          <c:x val="0.27835323292460884"/>
+          <c:y val="5.308157599652448E-2"/>
           <c:w val="0.49058708774509113"/>
           <c:h val="0.91237748169564881"/>
         </c:manualLayout>
@@ -558,6 +570,54 @@
               </c:ext>
             </c:extLst>
           </c:dPt>
+          <c:dPt>
+            <c:idx val="12"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1">
+                  <a:lumMod val="80000"/>
+                  <a:lumOff val="20000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln>
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst>
+                <a:outerShdw blurRad="254000" sx="102000" sy="102000" algn="ctr" rotWithShape="0">
+                  <a:prstClr val="black">
+                    <a:alpha val="20000"/>
+                  </a:prstClr>
+                </a:outerShdw>
+              </a:effectLst>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="13"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2">
+                  <a:lumMod val="80000"/>
+                  <a:lumOff val="20000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln>
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst>
+                <a:outerShdw blurRad="254000" sx="102000" sy="102000" algn="ctr" rotWithShape="0">
+                  <a:prstClr val="black">
+                    <a:alpha val="20000"/>
+                  </a:prstClr>
+                </a:outerShdw>
+              </a:effectLst>
+            </c:spPr>
+          </c:dPt>
           <c:dLbls>
             <c:spPr>
               <a:pattFill prst="pct75">
@@ -630,9 +690,9 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$B$8:$B$19</c:f>
+              <c:f>Sheet1!$B$8:$B$21</c:f>
               <c:strCache>
-                <c:ptCount val="12"/>
+                <c:ptCount val="14"/>
                 <c:pt idx="0">
                   <c:v>BATTERY</c:v>
                 </c:pt>
@@ -668,16 +728,22 @@
                 </c:pt>
                 <c:pt idx="11">
                   <c:v>WEATHER</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>AIR QUALITY</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>ATMOSPHERE</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$D$8:$D$19</c:f>
+              <c:f>Sheet1!$D$8:$D$21</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="12"/>
+                <c:ptCount val="14"/>
                 <c:pt idx="0">
                   <c:v>1426</c:v>
                 </c:pt>
@@ -713,6 +779,12 @@
                 </c:pt>
                 <c:pt idx="11">
                   <c:v>1654</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>1517</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>1928</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -749,10 +821,10 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.79752272438117588"/>
-          <c:y val="0.1204639614517567"/>
+          <c:x val="0.80232211866590986"/>
+          <c:y val="0.10305535186543119"/>
           <c:w val="0.18926227647149643"/>
-          <c:h val="0.76768063208760495"/>
+          <c:h val="0.80483492324923189"/>
         </c:manualLayout>
       </c:layout>
       <c:overlay val="0"/>
@@ -1498,14 +1570,14 @@
     <xdr:from>
       <xdr:col>7</xdr:col>
       <xdr:colOff>340179</xdr:colOff>
-      <xdr:row>4</xdr:row>
-      <xdr:rowOff>19050</xdr:rowOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>95249</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>16</xdr:col>
       <xdr:colOff>159204</xdr:colOff>
       <xdr:row>19</xdr:row>
-      <xdr:rowOff>14287</xdr:rowOff>
+      <xdr:rowOff>14286</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1603,9 +1675,9 @@
   <xdr:oneCellAnchor>
     <xdr:from>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>310244</xdr:colOff>
+      <xdr:colOff>317571</xdr:colOff>
       <xdr:row>6</xdr:row>
-      <xdr:rowOff>66675</xdr:rowOff>
+      <xdr:rowOff>59348</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="1475013" cy="2013628"/>
     <xdr:sp macro="" textlink="">
@@ -1621,7 +1693,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="6422573" y="1209675"/>
+          <a:off x="6420898" y="1202348"/>
           <a:ext cx="1475013" cy="2013628"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -1676,7 +1748,7 @@
               <a:ea typeface="Open Sans Semibold" panose="020B0706030804020204" pitchFamily="34" charset="0"/>
               <a:cs typeface="Open Sans Semibold" panose="020B0706030804020204" pitchFamily="34" charset="0"/>
             </a:rPr>
-            <a:t>15 000</a:t>
+            <a:t>17 500</a:t>
           </a:r>
         </a:p>
         <a:p>
@@ -1736,7 +1808,7 @@
               <a:ea typeface="Open Sans Semibold" panose="020B0706030804020204" pitchFamily="34" charset="0"/>
               <a:cs typeface="Open Sans Semibold" panose="020B0706030804020204" pitchFamily="34" charset="0"/>
             </a:rPr>
-            <a:t>12</a:t>
+            <a:t>14</a:t>
           </a:r>
         </a:p>
         <a:p>
@@ -1766,7 +1838,7 @@
               <a:ea typeface="Open Sans Semibold" panose="020B0706030804020204" pitchFamily="34" charset="0"/>
               <a:cs typeface="Open Sans Semibold" panose="020B0706030804020204" pitchFamily="34" charset="0"/>
             </a:rPr>
-            <a:t>5H 33M 9S</a:t>
+            <a:t>6H 30M 34S</a:t>
           </a:r>
           <a:endParaRPr lang="en-GB" sz="1000">
             <a:solidFill>
@@ -2081,10 +2153,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D59F4E39-D49C-4F18-99E0-EC8E072B42B6}">
-  <dimension ref="B2:D19"/>
+  <dimension ref="B2:D21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" zoomScale="340" zoomScaleNormal="340" workbookViewId="0">
-      <selection activeCell="F22" sqref="F22"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2099,12 +2171,12 @@
         <v>0</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>1</v>
+        <v>35</v>
       </c>
     </row>
     <row r="3" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C3">
         <v>1250</v>
@@ -2112,7 +2184,7 @@
     </row>
     <row r="4" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C4">
         <v>12</v>
@@ -2120,29 +2192,29 @@
     </row>
     <row r="5" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>5</v>
+        <v>31</v>
       </c>
     </row>
     <row r="7" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C7" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="D7" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="8" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C8" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="D8">
         <v>1426</v>
@@ -2150,10 +2222,10 @@
     </row>
     <row r="9" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C9" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="D9">
         <v>1934</v>
@@ -2161,10 +2233,10 @@
     </row>
     <row r="10" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C10" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="D10">
         <v>1643</v>
@@ -2172,10 +2244,10 @@
     </row>
     <row r="11" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C11" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="D11">
         <v>2222</v>
@@ -2183,10 +2255,10 @@
     </row>
     <row r="12" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C12" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="D12">
         <v>1674</v>
@@ -2194,10 +2266,10 @@
     </row>
     <row r="13" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C13" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="D13">
         <v>1850</v>
@@ -2205,10 +2277,10 @@
     </row>
     <row r="14" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C14" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="D14">
         <v>1817</v>
@@ -2216,10 +2288,10 @@
     </row>
     <row r="15" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C15" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="D15">
         <v>1401</v>
@@ -2227,10 +2299,10 @@
     </row>
     <row r="16" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C16" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="D16">
         <v>1536</v>
@@ -2238,10 +2310,10 @@
     </row>
     <row r="17" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C17" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="D17">
         <v>1350</v>
@@ -2249,10 +2321,10 @@
     </row>
     <row r="18" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C18" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="D18">
         <v>1482</v>
@@ -2260,13 +2332,35 @@
     </row>
     <row r="19" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C19" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="D19">
         <v>1654</v>
+      </c>
+    </row>
+    <row r="20" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B20" t="s">
+        <v>32</v>
+      </c>
+      <c r="C20" t="s">
+        <v>33</v>
+      </c>
+      <c r="D20">
+        <v>1517</v>
+      </c>
+    </row>
+    <row r="21" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B21" t="s">
+        <v>36</v>
+      </c>
+      <c r="C21" t="s">
+        <v>34</v>
+      </c>
+      <c r="D21">
+        <v>1928</v>
       </c>
     </row>
   </sheetData>

</xml_diff>